<commit_message>
* v1.1.0 Added visual comparison plots. Added formal colocalization test.
</commit_message>
<xml_diff>
--- a/targets/targets.xlsx
+++ b/targets/targets.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swvanderlaan/PLINK/analyses/stroke/AAO_IschemicStroke.git/targets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D1753-585E-194F-A83D-A3E727A141E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33248F94-1920-C24D-B017-7A4F8466B3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3500" windowWidth="27640" windowHeight="16780" xr2:uid="{26E516C3-6C7E-6B40-A40D-487B1BB2FD9A}"/>
+    <workbookView xWindow="10080" yWindow="5920" windowWidth="27640" windowHeight="16780" activeTab="2" xr2:uid="{26E516C3-6C7E-6B40-A40D-487B1BB2FD9A}"/>
   </bookViews>
   <sheets>
     <sheet name="TopLoci" sheetId="1" r:id="rId1"/>
-    <sheet name="Top_Combined" sheetId="2" r:id="rId2"/>
-    <sheet name="Top_Men" sheetId="3" r:id="rId3"/>
-    <sheet name="Top_Women" sheetId="4" r:id="rId4"/>
+    <sheet name="Clump_TRIB3" sheetId="5" r:id="rId2"/>
+    <sheet name="APOE" sheetId="6" r:id="rId3"/>
+    <sheet name="Top_Combined" sheetId="2" r:id="rId4"/>
+    <sheet name="Top_Men" sheetId="3" r:id="rId5"/>
+    <sheet name="Top_Women" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="341">
   <si>
     <t>SNP</t>
   </si>
@@ -812,6 +814,255 @@
   </si>
   <si>
     <t>rsID</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>RSQ</t>
+  </si>
+  <si>
+    <t>rs34353262</t>
+  </si>
+  <si>
+    <t>rs6107255</t>
+  </si>
+  <si>
+    <t>rs8120854</t>
+  </si>
+  <si>
+    <t>rs78880381</t>
+  </si>
+  <si>
+    <t>rs6051637</t>
+  </si>
+  <si>
+    <t>rs62191444</t>
+  </si>
+  <si>
+    <t>rs9941773</t>
+  </si>
+  <si>
+    <t>rs9941733</t>
+  </si>
+  <si>
+    <t>rs6084311</t>
+  </si>
+  <si>
+    <t>rs6037522</t>
+  </si>
+  <si>
+    <t>rs6037524</t>
+  </si>
+  <si>
+    <t>rs6051701</t>
+  </si>
+  <si>
+    <t>rs147711004</t>
+  </si>
+  <si>
+    <t>rs41289512</t>
+  </si>
+  <si>
+    <t>rs146275714</t>
+  </si>
+  <si>
+    <t>rs3745150</t>
+  </si>
+  <si>
+    <t>rs147636938</t>
+  </si>
+  <si>
+    <t>rs12972156</t>
+  </si>
+  <si>
+    <t>rs12972970</t>
+  </si>
+  <si>
+    <t>rs34342646</t>
+  </si>
+  <si>
+    <t>rs283811</t>
+  </si>
+  <si>
+    <t>rs283815</t>
+  </si>
+  <si>
+    <t>rs6857</t>
+  </si>
+  <si>
+    <t>rs71352238</t>
+  </si>
+  <si>
+    <t>rs184017</t>
+  </si>
+  <si>
+    <t>rs157580</t>
+  </si>
+  <si>
+    <t>rs2075650</t>
+  </si>
+  <si>
+    <t>rs157581</t>
+  </si>
+  <si>
+    <t>rs34095326</t>
+  </si>
+  <si>
+    <t>rs34404554</t>
+  </si>
+  <si>
+    <t>rs11556505</t>
+  </si>
+  <si>
+    <t>rs157582</t>
+  </si>
+  <si>
+    <t>rs59007384</t>
+  </si>
+  <si>
+    <t>rs77301115</t>
+  </si>
+  <si>
+    <t>rs116881820</t>
+  </si>
+  <si>
+    <t>rs79398853</t>
+  </si>
+  <si>
+    <t>rs2238681</t>
+  </si>
+  <si>
+    <t>rs75687619</t>
+  </si>
+  <si>
+    <t>rs76366838</t>
+  </si>
+  <si>
+    <t>rs114536010</t>
+  </si>
+  <si>
+    <t>rs8106922</t>
+  </si>
+  <si>
+    <t>rs118170342</t>
+  </si>
+  <si>
+    <t>rs34878901</t>
+  </si>
+  <si>
+    <t>rs115881343</t>
+  </si>
+  <si>
+    <t>rs1160985</t>
+  </si>
+  <si>
+    <t>rs760136</t>
+  </si>
+  <si>
+    <t>rs741780</t>
+  </si>
+  <si>
+    <t>rs112019714</t>
+  </si>
+  <si>
+    <t>rs1038025</t>
+  </si>
+  <si>
+    <t>rs1038026</t>
+  </si>
+  <si>
+    <t>rs1305062</t>
+  </si>
+  <si>
+    <t>rs10119</t>
+  </si>
+  <si>
+    <t>rs7259620</t>
+  </si>
+  <si>
+    <t>rs440446</t>
+  </si>
+  <si>
+    <t>rs769449</t>
+  </si>
+  <si>
+    <t>rs769450</t>
+  </si>
+  <si>
+    <t>rs1081105</t>
+  </si>
+  <si>
+    <t>rs75627662</t>
+  </si>
+  <si>
+    <t>rs439401</t>
+  </si>
+  <si>
+    <t>rs10414043</t>
+  </si>
+  <si>
+    <t>rs7256200</t>
+  </si>
+  <si>
+    <t>rs483082</t>
+  </si>
+  <si>
+    <t>rs59325138</t>
+  </si>
+  <si>
+    <t>rs584007</t>
+  </si>
+  <si>
+    <t>rs438811</t>
+  </si>
+  <si>
+    <t>rs12691088</t>
+  </si>
+  <si>
+    <t>rs5117</t>
+  </si>
+  <si>
+    <t>rs3826688</t>
+  </si>
+  <si>
+    <t>rs3925681</t>
+  </si>
+  <si>
+    <t>rs150966173</t>
+  </si>
+  <si>
+    <t>rs12721046</t>
+  </si>
+  <si>
+    <t>rs140480140</t>
+  </si>
+  <si>
+    <t>rs484195</t>
+  </si>
+  <si>
+    <t>rs56131196</t>
+  </si>
+  <si>
+    <t>rs814573</t>
+  </si>
+  <si>
+    <t>rs157592</t>
+  </si>
+  <si>
+    <t>rs157594</t>
+  </si>
+  <si>
+    <t>rs157595</t>
+  </si>
+  <si>
+    <t>rs111789331</t>
+  </si>
+  <si>
+    <t>rs66626994</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28047563-1103-AC49-A3BD-F706590F9E12}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1230,6 +1481,1080 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA8B37F-404B-264E-B2E0-C3259AA9F792}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.7E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3">
+        <v>-10500</v>
+      </c>
+      <c r="C3">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4">
+        <v>-3120</v>
+      </c>
+      <c r="C4">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="D4">
+        <v>4.6000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5">
+        <v>-2980</v>
+      </c>
+      <c r="C5">
+        <v>0.434</v>
+      </c>
+      <c r="D5">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6">
+        <v>-2980</v>
+      </c>
+      <c r="C6">
+        <v>0.434</v>
+      </c>
+      <c r="D6">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7">
+        <v>-2790</v>
+      </c>
+      <c r="C7">
+        <v>0.107</v>
+      </c>
+      <c r="D7">
+        <v>6.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8">
+        <v>-1100</v>
+      </c>
+      <c r="C8">
+        <v>0.748</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.8E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9">
+        <v>-927</v>
+      </c>
+      <c r="C9">
+        <v>0.748</v>
+      </c>
+      <c r="D9">
+        <v>3.6000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10">
+        <v>-702</v>
+      </c>
+      <c r="C10">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4.8999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11">
+        <v>-379</v>
+      </c>
+      <c r="C11">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="D11" s="2">
+        <v>8.6999999999999998E-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12">
+        <v>-324</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.8000000000000003E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13">
+        <v>182</v>
+      </c>
+      <c r="C13">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="D13">
+        <v>5.9000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14">
+        <v>343</v>
+      </c>
+      <c r="C14">
+        <v>0.623</v>
+      </c>
+      <c r="D14" s="2">
+        <v>9.0999999999999993E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15">
+        <v>4170</v>
+      </c>
+      <c r="C15">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="D15">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16">
+        <v>4210</v>
+      </c>
+      <c r="C16">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="D16">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17">
+        <v>4220</v>
+      </c>
+      <c r="C17">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18">
+        <v>324</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3.8000000000000003E-8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04032D6A-691C-634A-AB5D-F712F1848FD2}">
+  <dimension ref="A1:C72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2">
+        <v>-74023</v>
+      </c>
+      <c r="C2">
+        <v>0.102462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3">
+        <v>-60425</v>
+      </c>
+      <c r="C3">
+        <v>0.12436899999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4">
+        <v>-46494</v>
+      </c>
+      <c r="C4">
+        <v>0.121821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5">
+        <v>-26182</v>
+      </c>
+      <c r="C5">
+        <v>0.115425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6">
+        <v>-25307</v>
+      </c>
+      <c r="C6">
+        <v>0.15857399999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7">
+        <v>-24482</v>
+      </c>
+      <c r="C7">
+        <v>0.44341799999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8">
+        <v>-24345</v>
+      </c>
+      <c r="C8">
+        <v>0.44341799999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9">
+        <v>-23811</v>
+      </c>
+      <c r="C9">
+        <v>0.43671199999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10">
+        <v>-23441</v>
+      </c>
+      <c r="C10">
+        <v>0.48532700000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11">
+        <v>-21608</v>
+      </c>
+      <c r="C11">
+        <v>0.50449500000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12">
+        <v>-19687</v>
+      </c>
+      <c r="C12">
+        <v>0.68976800000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13">
+        <v>-17605</v>
+      </c>
+      <c r="C13">
+        <v>0.46330700000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14">
+        <v>-16972</v>
+      </c>
+      <c r="C14">
+        <v>0.52057600000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15">
+        <v>-16675</v>
+      </c>
+      <c r="C15">
+        <v>0.10673100000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>287</v>
+      </c>
+      <c r="B16">
+        <v>-16322</v>
+      </c>
+      <c r="C16">
+        <v>0.48396299999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>288</v>
+      </c>
+      <c r="B17">
+        <v>-16227</v>
+      </c>
+      <c r="C17">
+        <v>0.52057600000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18">
+        <v>-16097</v>
+      </c>
+      <c r="C18">
+        <v>0.29236000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B19">
+        <v>-16032</v>
+      </c>
+      <c r="C19">
+        <v>0.48396299999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>291</v>
+      </c>
+      <c r="B20">
+        <v>-15797</v>
+      </c>
+      <c r="C20">
+        <v>0.48396299999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21">
+        <v>-15722</v>
+      </c>
+      <c r="C21">
+        <v>0.52394499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>293</v>
+      </c>
+      <c r="B22">
+        <v>-15276</v>
+      </c>
+      <c r="C22">
+        <v>0.64044699999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23">
+        <v>-14968</v>
+      </c>
+      <c r="C23">
+        <v>0.170734</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24">
+        <v>-13989</v>
+      </c>
+      <c r="C24">
+        <v>0.15923699999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>296</v>
+      </c>
+      <c r="B25">
+        <v>-13156</v>
+      </c>
+      <c r="C25">
+        <v>0.15923699999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>297</v>
+      </c>
+      <c r="B26">
+        <v>-13124</v>
+      </c>
+      <c r="C26">
+        <v>0.126253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27">
+        <v>-12597</v>
+      </c>
+      <c r="C27">
+        <v>0.15923699999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B28">
+        <v>-12045</v>
+      </c>
+      <c r="C28">
+        <v>0.14686299999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>300</v>
+      </c>
+      <c r="B29">
+        <v>-11216</v>
+      </c>
+      <c r="C29">
+        <v>0.15923699999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>301</v>
+      </c>
+      <c r="B30">
+        <v>-10275</v>
+      </c>
+      <c r="C30">
+        <v>0.126774</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>302</v>
+      </c>
+      <c r="B31">
+        <v>-10073</v>
+      </c>
+      <c r="C31">
+        <v>0.11713800000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B32">
+        <v>-9464</v>
+      </c>
+      <c r="C32">
+        <v>0.126253</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>304</v>
+      </c>
+      <c r="B33">
+        <v>-8725</v>
+      </c>
+      <c r="C33">
+        <v>0.15923699999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>305</v>
+      </c>
+      <c r="B34">
+        <v>-8529</v>
+      </c>
+      <c r="C34">
+        <v>0.14794399999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>306</v>
+      </c>
+      <c r="B35">
+        <v>-8083</v>
+      </c>
+      <c r="C35">
+        <v>0.14794399999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B36">
+        <v>-7510</v>
+      </c>
+      <c r="C36">
+        <v>0.14072999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>308</v>
+      </c>
+      <c r="B37">
+        <v>-7084</v>
+      </c>
+      <c r="C37">
+        <v>0.15923699999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38">
+        <v>-6969</v>
+      </c>
+      <c r="C38">
+        <v>0.14794399999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>310</v>
+      </c>
+      <c r="B39">
+        <v>-6879</v>
+      </c>
+      <c r="C39">
+        <v>0.14794399999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>311</v>
+      </c>
+      <c r="B40">
+        <v>-6420</v>
+      </c>
+      <c r="C40">
+        <v>0.126774</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>312</v>
+      </c>
+      <c r="B41">
+        <v>-5268</v>
+      </c>
+      <c r="C41">
+        <v>0.41529899999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>313</v>
+      </c>
+      <c r="B42">
+        <v>-4153</v>
+      </c>
+      <c r="C42">
+        <v>0.14794399999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>314</v>
+      </c>
+      <c r="B43">
+        <v>-2774</v>
+      </c>
+      <c r="C43">
+        <v>0.10084600000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>315</v>
+      </c>
+      <c r="B44">
+        <v>-1939</v>
+      </c>
+      <c r="C44">
+        <v>0.76603299999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>316</v>
+      </c>
+      <c r="B45">
+        <v>-1497</v>
+      </c>
+      <c r="C45">
+        <v>0.12834699999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>317</v>
+      </c>
+      <c r="B47">
+        <v>1014</v>
+      </c>
+      <c r="C47">
+        <v>0.17324100000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>318</v>
+      </c>
+      <c r="B48">
+        <v>1635</v>
+      </c>
+      <c r="C48">
+        <v>0.44977200000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>319</v>
+      </c>
+      <c r="B49">
+        <v>2510</v>
+      </c>
+      <c r="C49">
+        <v>0.10906</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>320</v>
+      </c>
+      <c r="B50">
+        <v>3772</v>
+      </c>
+      <c r="C50">
+        <v>0.758517</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>321</v>
+      </c>
+      <c r="B51">
+        <v>3994</v>
+      </c>
+      <c r="C51">
+        <v>0.75112000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>322</v>
+      </c>
+      <c r="B52">
+        <v>4237</v>
+      </c>
+      <c r="C52">
+        <v>0.63435799999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>323</v>
+      </c>
+      <c r="B53">
+        <v>4350</v>
+      </c>
+      <c r="C53">
+        <v>0.11776399999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>324</v>
+      </c>
+      <c r="B54">
+        <v>4537</v>
+      </c>
+      <c r="C54">
+        <v>0.107658</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>325</v>
+      </c>
+      <c r="B55">
+        <v>4800</v>
+      </c>
+      <c r="C55">
+        <v>0.63435799999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>326</v>
+      </c>
+      <c r="B56">
+        <v>6545</v>
+      </c>
+      <c r="C56">
+        <v>0.121821</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>327</v>
+      </c>
+      <c r="B57">
+        <v>6849</v>
+      </c>
+      <c r="C57">
+        <v>0.62382000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>328</v>
+      </c>
+      <c r="B58">
+        <v>7020</v>
+      </c>
+      <c r="C58">
+        <v>0.107658</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>329</v>
+      </c>
+      <c r="B59">
+        <v>9159</v>
+      </c>
+      <c r="C59">
+        <v>0.118671</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>330</v>
+      </c>
+      <c r="B60">
+        <v>9263</v>
+      </c>
+      <c r="C60">
+        <v>0.15350900000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>331</v>
+      </c>
+      <c r="B61">
+        <v>9313</v>
+      </c>
+      <c r="C61">
+        <v>0.49268099999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>332</v>
+      </c>
+      <c r="B62">
+        <v>9709</v>
+      </c>
+      <c r="C62">
+        <v>0.15350900000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>333</v>
+      </c>
+      <c r="B63">
+        <v>9936</v>
+      </c>
+      <c r="C63">
+        <v>0.109224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>255</v>
+      </c>
+      <c r="B64">
+        <v>10219</v>
+      </c>
+      <c r="C64">
+        <v>0.68597699999999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>334</v>
+      </c>
+      <c r="B65">
+        <v>10905</v>
+      </c>
+      <c r="C65">
+        <v>0.68597699999999995</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>256</v>
+      </c>
+      <c r="B66">
+        <v>11005</v>
+      </c>
+      <c r="C66">
+        <v>0.68597699999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>335</v>
+      </c>
+      <c r="B67">
+        <v>12410</v>
+      </c>
+      <c r="C67">
+        <v>0.66228699999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>336</v>
+      </c>
+      <c r="B68">
+        <v>12573</v>
+      </c>
+      <c r="C68">
+        <v>0.63889200000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>337</v>
+      </c>
+      <c r="B69">
+        <v>13234</v>
+      </c>
+      <c r="C69">
+        <v>0.109707</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>338</v>
+      </c>
+      <c r="B70">
+        <v>13519</v>
+      </c>
+      <c r="C70">
+        <v>0.109224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71">
+        <v>15184</v>
+      </c>
+      <c r="C71">
+        <v>0.48630200000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>340</v>
+      </c>
+      <c r="B72">
+        <v>16293</v>
+      </c>
+      <c r="C72">
+        <v>0.48630200000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66CB7D6-C04E-8542-AAC8-76555C733E5A}">
   <dimension ref="A1:L58"/>
   <sheetViews>
@@ -3451,7 +4776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A91053-2224-B740-A9D9-65EDB67CA50D}">
   <dimension ref="A1:L141"/>
   <sheetViews>
@@ -8827,7 +10152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE36D56A-4D40-DA49-AFF6-2B305831E1CA}">
   <dimension ref="A1:L43"/>
   <sheetViews>

</xml_diff>